<commit_message>
Updated manda user to profile
</commit_message>
<xml_diff>
--- a/OrangeHRM_Test_Cases.xlsx
+++ b/OrangeHRM_Test_Cases.xlsx
@@ -569,7 +569,7 @@
 </t>
   </si>
   <si>
-    <t>1. Click on 'Manda User' Dropmenu 
+    <t>1. Click on 'Profile' Dropmenu 
 2. Select 'Logout' option (Verify ER-1)
 3. Click on 'Continue' button (Verify ER-2)</t>
   </si>
@@ -597,7 +597,7 @@
     <t>Validate logging out and browsing back</t>
   </si>
   <si>
-    <t>1. Click on 'Manda User' Dropmenu 
+    <t>1. Click on 'Profile' Dropmenu 
 2. Select 'Logout' option
 3. Click on Browser back button (Verify ER-1)</t>
   </si>
@@ -617,7 +617,7 @@
 </t>
   </si>
   <si>
-    <t>1. Click on 'Manda User' Dropmenu in Firefox Browser
+    <t>1. Click on 'Profile' Dropmenu in Firefox Browser
 2. Select 'Logout' option
 3. Perform any operation which requires the user to log, say navigating to Address Book page in the Chrome Browser of Mobile device (Verify ER-1)</t>
   </si>
@@ -631,7 +631,7 @@
     <t xml:space="preserve">Validate logging out and loggin in immediately after logout </t>
   </si>
   <si>
-    <t>1. Click on 'Manda User' Dropmenu 
+    <t>1. Click on 'Profile' Dropmenu 
 2. Select 'Logout' option
 3. Login immediately again with same or different account (Verify ER-1)</t>
   </si>
@@ -649,7 +649,7 @@
 2. User is logged in</t>
   </si>
   <si>
-    <t>1. Click on 'Manda User' Dropmenu 
+    <t>1. Click on 'Profile' Dropmenu 
 2. Select 'Logout' option
 3. Check the Page Heading, Page Title, Page URL and Breadcrumb of the displayed 'Account Logout' page (Verify ER-1)</t>
   </si>
@@ -663,7 +663,7 @@
     <t>Validate the UI of the Logout option and the 'Account Logout' page</t>
   </si>
   <si>
-    <t>1. Click on 'Manda User' Dropmenu 
+    <t>1. Click on 'Profile' Dropmenu 
 2. Select 'Logout' option (Verify ER-1)</t>
   </si>
   <si>
@@ -2158,8 +2158,8 @@
   <sheetPr/>
   <dimension ref="A1:Z998"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A1" sqref="A$1:A$1048576"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5"/>
@@ -30451,8 +30451,8 @@
   <sheetPr/>
   <dimension ref="A1:K10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="64" zoomScaleNormal="64" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" zoomScale="64" zoomScaleNormal="64" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>

</xml_diff>

<commit_message>
Test cases added till location function yet to add the company search test cases
</commit_message>
<xml_diff>
--- a/OrangeHRM_Test_Cases.xlsx
+++ b/OrangeHRM_Test_Cases.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="460" uniqueCount="308">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="492" uniqueCount="330">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -1357,6 +1357,121 @@
   <si>
     <t xml:space="preserve">1. System should ask to fill the  required fields.
 </t>
+  </si>
+  <si>
+    <t>TC_AF_033</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Validate the "Locations"functionality with all valid inputs.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. click on the 'Admin' button from the left sidebar.
+2. Click on Organizations&gt;Locations&gt;"+Add"
+3.Input valid name of organization whom are are going use the software.. 
+4.Input valid citty name in the "City" field. 
+5. Input the valid state/province.
+6. INput valid zip/postal code. 
+7. Select the country of the organization.
+8. Input valid phone number. 
+9. Input valid fax number. 
+10. Input valid address. 
+11. Input a note in the "Note" field.
+12.. Click on the 'Save' button. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Company name &amp; location should save successfully in the system. </t>
+  </si>
+  <si>
+    <t>TC_AF_034</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Validate the "Locations"functionality with all invalid inputs.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. click on the 'Admin' button from the left sidebar.
+2. Click on Organizations&gt;Locations&gt;"+Add"
+3.Input Invalid name of organization whom are are going use the software.. 
+4.Input Invalid citty name in the "City" field. 
+5. Input the Invalid state/province.
+6. INput Invalid zip/postal code. 
+7. Select the country of the organization.
+8. Input Invalid phone number. 
+9. Input Invalid fax number. 
+10. Input Invalid address. 
+11. Input a note in the "Note" field.
+12.. Click on the 'Save' button. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. System should not allow any invalid company to register. </t>
+  </si>
+  <si>
+    <t>TC_AF_035</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Validate the "Locations"functionality with all irrelevant inputs.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. click on the 'Admin' button from the left sidebar.
+2. Click on Organizations&gt;Locations&gt;"+Add"
+3.Input digits of in the "Name" field. 
+4.Input digits in the "City" field. 
+5. Input digits in the state/province field. 
+6. Input a word or name in the  zip/postal code field. 
+7. Select the country of the organization.
+8. Input word or name in the phone number field.  
+9. Input word or name in the fax number field.
+10. Input digits in the address field.
+11. Input a numerical note in the "Note" field.
+12.. Click on the 'Save' button. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. System should not allow to register any compnay or locations which is totally irrelevant. 
+</t>
+  </si>
+  <si>
+    <t>TC_AF_036</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Validate the "Locations"functionality with all empty fields.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. click on the 'Admin' button from the left sidebar.
+2. Click on Organizations&gt;Locations&gt;"+Add"
+3.Input nothing of in the "Name" field. 
+4.Input notthing in the "City" field. 
+5. Input nothing in the state/province field. 
+6. Input nothing in the  zip/postal code field. 
+7. Select the country of the organization.
+8. Input nothing in the phone number field.  
+9. Input nothing in the fax number field.
+10. Input nothing in the address field.
+11. Input nothing in the "Note" field.
+12.. Click on the 'Save' button. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. System should show an error message or to ask required fields. </t>
+  </si>
+  <si>
+    <t>TC_AF_037</t>
+  </si>
+  <si>
+    <t>TC_AF_038</t>
+  </si>
+  <si>
+    <t>TC_AF_039</t>
+  </si>
+  <si>
+    <t>TC_AF_040</t>
+  </si>
+  <si>
+    <t>TC_AF_041</t>
+  </si>
+  <si>
+    <t>TC_AF_042</t>
   </si>
 </sst>
 </file>
@@ -31475,10 +31590,10 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:K33"/>
+  <dimension ref="A1:K43"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="87" zoomScaleNormal="87" topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="F35" sqref="F35"/>
+    <sheetView tabSelected="1" zoomScale="87" zoomScaleNormal="87" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5"/>
@@ -32261,6 +32376,122 @@
         <v>307</v>
       </c>
     </row>
+    <row r="34" ht="409.5" spans="1:7">
+      <c r="A34" s="4" t="s">
+        <v>308</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="C34" s="9" t="s">
+        <v>309</v>
+      </c>
+      <c r="D34" s="6" t="s">
+        <v>157</v>
+      </c>
+      <c r="E34" s="7" t="s">
+        <v>310</v>
+      </c>
+      <c r="G34" s="9" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="35" ht="409.5" spans="1:7">
+      <c r="A35" s="4" t="s">
+        <v>312</v>
+      </c>
+      <c r="B35" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="C35" s="9" t="s">
+        <v>313</v>
+      </c>
+      <c r="D35" s="6" t="s">
+        <v>157</v>
+      </c>
+      <c r="E35" s="7" t="s">
+        <v>314</v>
+      </c>
+      <c r="G35" s="9" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="36" ht="409.5" spans="1:7">
+      <c r="A36" s="4" t="s">
+        <v>316</v>
+      </c>
+      <c r="B36" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="C36" s="9" t="s">
+        <v>317</v>
+      </c>
+      <c r="D36" s="6" t="s">
+        <v>157</v>
+      </c>
+      <c r="E36" s="7" t="s">
+        <v>318</v>
+      </c>
+      <c r="G36" s="9" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="37" ht="409.5" spans="1:7">
+      <c r="A37" s="4" t="s">
+        <v>320</v>
+      </c>
+      <c r="B37" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="C37" s="9" t="s">
+        <v>321</v>
+      </c>
+      <c r="D37" s="6" t="s">
+        <v>157</v>
+      </c>
+      <c r="E37" s="7" t="s">
+        <v>322</v>
+      </c>
+      <c r="G37" s="9" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="38" ht="26" spans="1:2">
+      <c r="A38" s="4" t="s">
+        <v>324</v>
+      </c>
+      <c r="B38" s="5" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="39" ht="26" spans="1:2">
+      <c r="A39" s="4" t="s">
+        <v>325</v>
+      </c>
+      <c r="B39" s="5" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1">
+      <c r="A40" s="4" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1">
+      <c r="A41" s="4" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1">
+      <c r="A42" s="4" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1">
+      <c r="A43" s="4" t="s">
+        <v>329</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>

<commit_message>
Test cases updated till Qualifications of Admin functionality
</commit_message>
<xml_diff>
--- a/OrangeHRM_Test_Cases.xlsx
+++ b/OrangeHRM_Test_Cases.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="492" uniqueCount="330">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="607" uniqueCount="406">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -1459,19 +1459,322 @@
     <t>TC_AF_037</t>
   </si>
   <si>
+    <t>Validate the "Add Skills" functionality with all valid inputs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. click on the 'Admin' button from the left sidebar.
+2. Click on Oualifications&gt;Skills&gt;"+Add"
+3.Input valid skill name in the "Name" field. 
+4.Input valid skill description in the "Description" field. 
+5. Click on the 'Save' button. </t>
+  </si>
+  <si>
+    <t>*Skill Name: Software Tester
+*Description: End to End software testing with test plan,test scenarios,test cases, test execution results,bug reports.</t>
+  </si>
+  <si>
+    <t>1. System should create the skill.</t>
+  </si>
+  <si>
     <t>TC_AF_038</t>
   </si>
   <si>
+    <t>Validate the "Add Skills" functionality with all invalid inputs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. click on the 'Admin' button from the left sidebar.
+2. Click on Oualifications&gt;Skills&gt;"+Add"
+3.Input invalid skill name in the "Name" field. 
+4.Input invalid skill description in the "Description" field. 
+5. Click on the 'Save' button. </t>
+  </si>
+  <si>
+    <t>*Skill Name: abc123
+*Description: djhfjdhdsjdjh</t>
+  </si>
+  <si>
+    <t>1. System will also create the invalid skills though nobody will use this skill.</t>
+  </si>
+  <si>
     <t>TC_AF_039</t>
   </si>
   <si>
+    <t>Validate the "Add Skills" functionality with all numeric inputs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. click on the 'Admin' button from the left sidebar.
+2. Click on Oualifications&gt;Skills&gt;"+Add"
+3.Input some digits in the "Name" field. 
+4.Input some digits in the "Description" field. 
+5. Click on the 'Save' button. </t>
+  </si>
+  <si>
+    <t>*Skill Name: 01234567
+*Description: 012345676</t>
+  </si>
+  <si>
+    <t>1. System should not allow such inputs.</t>
+  </si>
+  <si>
     <t>TC_AF_040</t>
   </si>
   <si>
+    <t xml:space="preserve">Validate the "Add Skills" functionality with only filling the "Name" Field. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. click on the 'Admin' button from the left sidebar.
+2. Click on Oualifications&gt;Skills&gt;"+Add"
+3.Input valid skill name in the "Name" field. 
+4.Input nothing in the "Description" field. 
+5. Click on the 'Save' button. </t>
+  </si>
+  <si>
+    <t>*Name- Cloud Engineer.</t>
+  </si>
+  <si>
+    <t>1. System should create the skill if already not existed without the description.</t>
+  </si>
+  <si>
     <t>TC_AF_041</t>
   </si>
   <si>
+    <t>Validate the "Add Skills" functionality keeping the all feilds empty.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. click on the 'Admin' button from the left sidebar.
+2. Click on Oualifications&gt;Skills&gt;"+Add"
+3.Input nothing in the "Name" field. 
+4.Input nothing in the "Description" field. 
+5. Click on the 'Save' button. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. System should ask for the skill name &amp; description
+ or pop up messege to input required fields.
+</t>
+  </si>
+  <si>
     <t>TC_AF_042</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Validate the "Add Education" functionality with all valid inputs.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. click on the 'Admin' button from the left sidebar.
+2. Click on Oualifications&gt;Skills&gt;"+Add"
+3.Input valid highest education level in the "Level" field. 
+4. Click on the 'Save' button. </t>
+  </si>
+  <si>
+    <t>*Name: Post-Graduation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. System should add add the education level if not added before to the system. 
+</t>
+  </si>
+  <si>
+    <t>TC_AF_043</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Validate the "Add Education" functionality with all invalid inputs.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. click on the 'Admin' button from the left sidebar.
+2. Click on Oualifications&gt;Skills&gt;"+Add"
+3.Input invalid highest education level in the "Level" field. 
+4. Click on the 'Save' button. </t>
+  </si>
+  <si>
+    <t>*Name: asf123</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. System will create the invalid education level too though nobody will use it. 
+</t>
+  </si>
+  <si>
+    <t>TC_AF_044</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Validate the "Add Education" functionality with input nothing in the fields. 
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. click on the 'Admin' button from the left sidebar.
+2. Click on Oualifications&gt;Skills&gt;"+Add"
+3.Input nothing in the "Level" field. 
+4. Click on the 'Save' button. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. System should ask for the inputs or pop up messege to input required fields.
+</t>
+  </si>
+  <si>
+    <t>TC_AF_045</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Validate "Add License" fields with valid inputs.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. click on the 'Admin' button from the left sidebar.
+2. Click on Oualifications&gt;Licenses&gt;"+Add"
+3.Input valid certification name in the "Name" field. 
+4. Click on the 'Save' button. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">*Name- Association of Chartered Certified Accountants(ACCA)
+</t>
+  </si>
+  <si>
+    <t>1. System should create the license/certification name.</t>
+  </si>
+  <si>
+    <t>TC_AF_046</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Validate "Add License" fields with invalid inputs.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. click on the 'Admin' button from the left sidebar.
+2. Click on Oualifications&gt;Licenses&gt;"+Add"
+3.Input invalid certification name in the "Name" field. 
+4. Click on the 'Save' button. </t>
+  </si>
+  <si>
+    <t>*Name: kjahjkdjsad12345jjdfkjdj(123jh)</t>
+  </si>
+  <si>
+    <t>1. System will also create the invalid license/certification name.</t>
+  </si>
+  <si>
+    <t>TC_AF_047</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Validate "Add License" functionality with empty fields.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. click on the 'Admin' button from the left sidebar.
+2. Click on Oualifications&gt;Licenses&gt;"+Add"
+3.Input nothing in the "Name" field. 
+4. Click on the 'Save' button. </t>
+  </si>
+  <si>
+    <t>TC_AF_048</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Validate the "Add Language" functionality with valid inputs.
+ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. click on the 'Admin' button from the left sidebar.
+2. Click on Oualifications&gt;Language&gt;"+Add"
+3.Input valid language name in the "Name" field. 
+4. Click on the 'Save' button. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">*Name- Bengali </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. System should create the language name if not added previously. </t>
+  </si>
+  <si>
+    <t>TC_AF_049</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Validate the "Add Language" functionality with invalid inputs.
+ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. click on the 'Admin' button from the left sidebar.
+2. Click on Oualifications&gt;Language&gt;"+Add"
+3.Input invalid language name in the "Name" field. 
+4. Click on the 'Save' button. </t>
+  </si>
+  <si>
+    <t>* Name: Ban34354</t>
+  </si>
+  <si>
+    <t>1. System will still add the inputs.</t>
+  </si>
+  <si>
+    <t>TC_AF_050</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Validate the "Add Language" functionality with empty fields.
+ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. click on the 'Admin' button from the left sidebar.
+2. Click on Oualifications&gt;Language&gt;"+Add"
+3.Input nothing in the "Name" field. 
+4. Click on the 'Save' button. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. System should ask for the inputs or pop up messege to input required fields.
+</t>
+  </si>
+  <si>
+    <t>TC_AF_051</t>
+  </si>
+  <si>
+    <t>Vaidate the "Add Membership" functionality with valid inputs.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. click on the 'Admin' button from the left sidebar.
+2. Click on Oualifications&gt;Memberships&gt;"+Add"
+3.Input valid membership name in the "Name" field. 
+4. Click on the 'Save' button. </t>
+  </si>
+  <si>
+    <t>*Name: ISTQB</t>
+  </si>
+  <si>
+    <t>1. System should add the membership if not added previously.</t>
+  </si>
+  <si>
+    <t>TC_AF_052</t>
+  </si>
+  <si>
+    <t>Vaidate the "Add Membership" functionality with invalid inputs.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. click on the 'Admin' button from the left sidebar.
+2. Click on Oualifications&gt;Memberships&gt;"+Add"
+3.Input invalid membership name in the "Name" field. 
+4. Click on the 'Save' button. </t>
+  </si>
+  <si>
+    <t>*Name: skjdjk7765r</t>
+  </si>
+  <si>
+    <t>TC_AF_053</t>
+  </si>
+  <si>
+    <t>Vaidate the "Add Membership" functionality with empty fields.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. click on the 'Admin' button from the left sidebar.
+2. Click on Oualifications&gt;Memberships&gt;"+Add"
+3.Input nothing in the "Name" field. 
+4. Click on the 'Save' button. </t>
+  </si>
+  <si>
+    <t>TC_AF_054</t>
+  </si>
+  <si>
+    <t>TC_AF_055</t>
+  </si>
+  <si>
+    <t>TC_AF_056</t>
+  </si>
+  <si>
+    <t>TC_AF_057</t>
+  </si>
+  <si>
+    <t>TC_AF_058</t>
   </si>
 </sst>
 </file>
@@ -31590,10 +31893,10 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:K43"/>
+  <dimension ref="A1:K59"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="87" zoomScaleNormal="87" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="C38" sqref="C38"/>
+    <sheetView tabSelected="1" zoomScale="87" zoomScaleNormal="87" topLeftCell="A54" workbookViewId="0">
+      <selection activeCell="E55" sqref="E55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5"/>
@@ -32004,7 +32307,7 @@
       <c r="F17" t="s">
         <v>232</v>
       </c>
-      <c r="G17" s="9" t="s">
+      <c r="G17" s="7" t="s">
         <v>233</v>
       </c>
     </row>
@@ -32027,7 +32330,7 @@
       <c r="F18" t="s">
         <v>237</v>
       </c>
-      <c r="G18" s="9" t="s">
+      <c r="G18" s="7" t="s">
         <v>238</v>
       </c>
     </row>
@@ -32050,7 +32353,7 @@
       <c r="F19" t="s">
         <v>242</v>
       </c>
-      <c r="G19" s="9" t="s">
+      <c r="G19" s="7" t="s">
         <v>243</v>
       </c>
     </row>
@@ -32073,7 +32376,7 @@
       <c r="F20" t="s">
         <v>193</v>
       </c>
-      <c r="G20" s="9" t="s">
+      <c r="G20" s="7" t="s">
         <v>247</v>
       </c>
     </row>
@@ -32096,7 +32399,7 @@
       <c r="F21" t="s">
         <v>251</v>
       </c>
-      <c r="G21" s="9" t="s">
+      <c r="G21" s="7" t="s">
         <v>252</v>
       </c>
     </row>
@@ -32119,7 +32422,7 @@
       <c r="F22" t="s">
         <v>256</v>
       </c>
-      <c r="G22" s="9" t="s">
+      <c r="G22" s="7" t="s">
         <v>257</v>
       </c>
     </row>
@@ -32142,7 +32445,7 @@
       <c r="F23" t="s">
         <v>261</v>
       </c>
-      <c r="G23" s="9" t="s">
+      <c r="G23" s="7" t="s">
         <v>262</v>
       </c>
     </row>
@@ -32165,7 +32468,7 @@
       <c r="F24" t="s">
         <v>193</v>
       </c>
-      <c r="G24" s="9" t="s">
+      <c r="G24" s="7" t="s">
         <v>247</v>
       </c>
     </row>
@@ -32185,10 +32488,10 @@
       <c r="E25" s="7" t="s">
         <v>268</v>
       </c>
-      <c r="F25" s="9" t="s">
+      <c r="F25" s="7" t="s">
         <v>269</v>
       </c>
-      <c r="G25" s="9" t="s">
+      <c r="G25" s="7" t="s">
         <v>270</v>
       </c>
     </row>
@@ -32208,10 +32511,10 @@
       <c r="E26" s="7" t="s">
         <v>273</v>
       </c>
-      <c r="F26" s="9" t="s">
+      <c r="F26" s="7" t="s">
         <v>274</v>
       </c>
-      <c r="G26" s="9" t="s">
+      <c r="G26" s="7" t="s">
         <v>275</v>
       </c>
     </row>
@@ -32234,7 +32537,7 @@
       <c r="F27" t="s">
         <v>242</v>
       </c>
-      <c r="G27" s="9" t="s">
+      <c r="G27" s="7" t="s">
         <v>279</v>
       </c>
     </row>
@@ -32257,7 +32560,7 @@
       <c r="F28" t="s">
         <v>193</v>
       </c>
-      <c r="G28" s="9" t="s">
+      <c r="G28" s="7" t="s">
         <v>283</v>
       </c>
     </row>
@@ -32277,10 +32580,10 @@
       <c r="E29" s="7" t="s">
         <v>286</v>
       </c>
-      <c r="F29" s="9" t="s">
+      <c r="F29" s="7" t="s">
         <v>287</v>
       </c>
-      <c r="G29" s="9" t="s">
+      <c r="G29" s="7" t="s">
         <v>288</v>
       </c>
     </row>
@@ -32300,10 +32603,10 @@
       <c r="E30" s="7" t="s">
         <v>291</v>
       </c>
-      <c r="F30" s="9" t="s">
+      <c r="F30" s="7" t="s">
         <v>292</v>
       </c>
-      <c r="G30" s="9" t="s">
+      <c r="G30" s="7" t="s">
         <v>293</v>
       </c>
     </row>
@@ -32323,10 +32626,10 @@
       <c r="E31" s="7" t="s">
         <v>296</v>
       </c>
-      <c r="F31" s="9" t="s">
+      <c r="F31" s="7" t="s">
         <v>297</v>
       </c>
-      <c r="G31" s="9" t="s">
+      <c r="G31" s="7" t="s">
         <v>298</v>
       </c>
     </row>
@@ -32346,10 +32649,10 @@
       <c r="E32" s="7" t="s">
         <v>301</v>
       </c>
-      <c r="F32" s="9" t="s">
+      <c r="F32" s="7" t="s">
         <v>302</v>
       </c>
-      <c r="G32" s="9" t="s">
+      <c r="G32" s="7" t="s">
         <v>303</v>
       </c>
     </row>
@@ -32372,7 +32675,7 @@
       <c r="F33" t="s">
         <v>193</v>
       </c>
-      <c r="G33" s="9" t="s">
+      <c r="G33" s="7" t="s">
         <v>307</v>
       </c>
     </row>
@@ -32383,7 +32686,7 @@
       <c r="B34" s="5" t="s">
         <v>155</v>
       </c>
-      <c r="C34" s="9" t="s">
+      <c r="C34" s="7" t="s">
         <v>309</v>
       </c>
       <c r="D34" s="6" t="s">
@@ -32392,7 +32695,7 @@
       <c r="E34" s="7" t="s">
         <v>310</v>
       </c>
-      <c r="G34" s="9" t="s">
+      <c r="G34" s="7" t="s">
         <v>311</v>
       </c>
     </row>
@@ -32403,7 +32706,7 @@
       <c r="B35" s="5" t="s">
         <v>155</v>
       </c>
-      <c r="C35" s="9" t="s">
+      <c r="C35" s="7" t="s">
         <v>313</v>
       </c>
       <c r="D35" s="6" t="s">
@@ -32412,7 +32715,7 @@
       <c r="E35" s="7" t="s">
         <v>314</v>
       </c>
-      <c r="G35" s="9" t="s">
+      <c r="G35" s="7" t="s">
         <v>315</v>
       </c>
     </row>
@@ -32423,7 +32726,7 @@
       <c r="B36" s="5" t="s">
         <v>155</v>
       </c>
-      <c r="C36" s="9" t="s">
+      <c r="C36" s="7" t="s">
         <v>317</v>
       </c>
       <c r="D36" s="6" t="s">
@@ -32432,7 +32735,7 @@
       <c r="E36" s="7" t="s">
         <v>318</v>
       </c>
-      <c r="G36" s="9" t="s">
+      <c r="G36" s="7" t="s">
         <v>319</v>
       </c>
     </row>
@@ -32443,53 +32746,431 @@
       <c r="B37" s="5" t="s">
         <v>155</v>
       </c>
-      <c r="C37" s="9" t="s">
+      <c r="C37" s="7" t="s">
         <v>321</v>
-      </c>
-      <c r="D37" s="6" t="s">
-        <v>157</v>
       </c>
       <c r="E37" s="7" t="s">
         <v>322</v>
       </c>
-      <c r="G37" s="9" t="s">
+      <c r="G37" s="7" t="s">
         <v>323</v>
       </c>
     </row>
-    <row r="38" ht="26" spans="1:2">
+    <row r="38" ht="203" spans="1:7">
       <c r="A38" s="4" t="s">
         <v>324</v>
       </c>
       <c r="B38" s="5" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="39" ht="26" spans="1:2">
+      <c r="C38" s="9" t="s">
+        <v>325</v>
+      </c>
+      <c r="D38" s="6" t="s">
+        <v>157</v>
+      </c>
+      <c r="E38" s="7" t="s">
+        <v>326</v>
+      </c>
+      <c r="F38" s="9" t="s">
+        <v>327</v>
+      </c>
+      <c r="G38" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="39" ht="203" spans="1:7">
       <c r="A39" s="4" t="s">
-        <v>325</v>
+        <v>329</v>
       </c>
       <c r="B39" s="5" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="40" spans="1:1">
+      <c r="C39" s="9" t="s">
+        <v>330</v>
+      </c>
+      <c r="D39" s="6" t="s">
+        <v>157</v>
+      </c>
+      <c r="E39" s="7" t="s">
+        <v>331</v>
+      </c>
+      <c r="F39" s="9" t="s">
+        <v>332</v>
+      </c>
+      <c r="G39" s="9" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="40" ht="188.5" spans="1:7">
       <c r="A40" s="4" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="41" spans="1:1">
+        <v>334</v>
+      </c>
+      <c r="B40" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="C40" s="9" t="s">
+        <v>335</v>
+      </c>
+      <c r="D40" s="6" t="s">
+        <v>157</v>
+      </c>
+      <c r="E40" s="7" t="s">
+        <v>336</v>
+      </c>
+      <c r="F40" s="9" t="s">
+        <v>337</v>
+      </c>
+      <c r="G40" s="9" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="41" ht="188.5" spans="1:7">
       <c r="A41" s="4" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="42" spans="1:1">
+        <v>339</v>
+      </c>
+      <c r="B41" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="C41" s="9" t="s">
+        <v>340</v>
+      </c>
+      <c r="D41" s="6" t="s">
+        <v>157</v>
+      </c>
+      <c r="E41" s="7" t="s">
+        <v>341</v>
+      </c>
+      <c r="F41" t="s">
+        <v>342</v>
+      </c>
+      <c r="G41" s="9" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="42" ht="174" spans="1:7">
       <c r="A42" s="4" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="43" spans="1:1">
+        <v>344</v>
+      </c>
+      <c r="B42" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="C42" s="9" t="s">
+        <v>345</v>
+      </c>
+      <c r="D42" s="6" t="s">
+        <v>157</v>
+      </c>
+      <c r="E42" s="7" t="s">
+        <v>346</v>
+      </c>
+      <c r="G42" s="9" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="43" ht="159.5" spans="1:7">
       <c r="A43" s="4" t="s">
-        <v>329</v>
+        <v>348</v>
+      </c>
+      <c r="B43" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="C43" s="9" t="s">
+        <v>349</v>
+      </c>
+      <c r="D43" s="6" t="s">
+        <v>157</v>
+      </c>
+      <c r="E43" s="7" t="s">
+        <v>350</v>
+      </c>
+      <c r="F43" t="s">
+        <v>351</v>
+      </c>
+      <c r="G43" s="9" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="44" ht="174" spans="1:7">
+      <c r="A44" s="4" t="s">
+        <v>353</v>
+      </c>
+      <c r="B44" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="C44" s="9" t="s">
+        <v>354</v>
+      </c>
+      <c r="D44" s="6" t="s">
+        <v>157</v>
+      </c>
+      <c r="E44" s="7" t="s">
+        <v>355</v>
+      </c>
+      <c r="F44" t="s">
+        <v>356</v>
+      </c>
+      <c r="G44" s="9" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="45" ht="145" spans="1:7">
+      <c r="A45" s="4" t="s">
+        <v>358</v>
+      </c>
+      <c r="B45" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="C45" s="9" t="s">
+        <v>359</v>
+      </c>
+      <c r="D45" s="6" t="s">
+        <v>157</v>
+      </c>
+      <c r="E45" s="7" t="s">
+        <v>360</v>
+      </c>
+      <c r="G45" s="9" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="46" ht="159.5" spans="1:8">
+      <c r="A46" s="4" t="s">
+        <v>362</v>
+      </c>
+      <c r="B46" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="C46" s="9" t="s">
+        <v>363</v>
+      </c>
+      <c r="D46" s="6" t="s">
+        <v>157</v>
+      </c>
+      <c r="E46" s="7" t="s">
+        <v>364</v>
+      </c>
+      <c r="F46" s="9" t="s">
+        <v>365</v>
+      </c>
+      <c r="G46" s="9" t="s">
+        <v>366</v>
+      </c>
+      <c r="H46" s="9"/>
+    </row>
+    <row r="47" ht="159.5" spans="1:7">
+      <c r="A47" s="4" t="s">
+        <v>367</v>
+      </c>
+      <c r="B47" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="C47" s="9" t="s">
+        <v>368</v>
+      </c>
+      <c r="D47" s="6" t="s">
+        <v>157</v>
+      </c>
+      <c r="E47" s="7" t="s">
+        <v>369</v>
+      </c>
+      <c r="F47" s="9" t="s">
+        <v>370</v>
+      </c>
+      <c r="G47" s="9" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="48" ht="145" spans="1:7">
+      <c r="A48" s="4" t="s">
+        <v>372</v>
+      </c>
+      <c r="B48" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="C48" s="9" t="s">
+        <v>373</v>
+      </c>
+      <c r="D48" s="6" t="s">
+        <v>157</v>
+      </c>
+      <c r="E48" s="7" t="s">
+        <v>374</v>
+      </c>
+      <c r="G48" s="9" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="49" ht="159.5" spans="1:7">
+      <c r="A49" s="4" t="s">
+        <v>375</v>
+      </c>
+      <c r="B49" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="C49" s="9" t="s">
+        <v>376</v>
+      </c>
+      <c r="D49" s="6" t="s">
+        <v>157</v>
+      </c>
+      <c r="E49" s="7" t="s">
+        <v>377</v>
+      </c>
+      <c r="F49" t="s">
+        <v>378</v>
+      </c>
+      <c r="G49" s="9" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="50" ht="159.5" spans="1:7">
+      <c r="A50" s="4" t="s">
+        <v>380</v>
+      </c>
+      <c r="B50" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="C50" s="9" t="s">
+        <v>381</v>
+      </c>
+      <c r="D50" s="6" t="s">
+        <v>157</v>
+      </c>
+      <c r="E50" s="7" t="s">
+        <v>382</v>
+      </c>
+      <c r="F50" t="s">
+        <v>383</v>
+      </c>
+      <c r="G50" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="51" ht="145" spans="1:7">
+      <c r="A51" s="4" t="s">
+        <v>385</v>
+      </c>
+      <c r="B51" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="C51" s="9" t="s">
+        <v>386</v>
+      </c>
+      <c r="D51" s="6" t="s">
+        <v>157</v>
+      </c>
+      <c r="E51" s="7" t="s">
+        <v>387</v>
+      </c>
+      <c r="G51" s="9" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="52" ht="159.5" spans="1:7">
+      <c r="A52" s="4" t="s">
+        <v>389</v>
+      </c>
+      <c r="B52" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="C52" s="9" t="s">
+        <v>390</v>
+      </c>
+      <c r="D52" s="6" t="s">
+        <v>157</v>
+      </c>
+      <c r="E52" s="7" t="s">
+        <v>391</v>
+      </c>
+      <c r="F52" t="s">
+        <v>392</v>
+      </c>
+      <c r="G52" s="9" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="53" ht="159.5" spans="1:7">
+      <c r="A53" s="4" t="s">
+        <v>394</v>
+      </c>
+      <c r="B53" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="C53" s="9" t="s">
+        <v>395</v>
+      </c>
+      <c r="D53" s="6" t="s">
+        <v>157</v>
+      </c>
+      <c r="E53" s="7" t="s">
+        <v>396</v>
+      </c>
+      <c r="F53" t="s">
+        <v>397</v>
+      </c>
+      <c r="G53" s="9" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="54" ht="145" spans="1:7">
+      <c r="A54" s="4" t="s">
+        <v>398</v>
+      </c>
+      <c r="B54" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="C54" s="9" t="s">
+        <v>399</v>
+      </c>
+      <c r="D54" s="6" t="s">
+        <v>157</v>
+      </c>
+      <c r="E54" s="7" t="s">
+        <v>400</v>
+      </c>
+      <c r="G54" s="9" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="55" ht="26" spans="1:2">
+      <c r="A55" s="4" t="s">
+        <v>401</v>
+      </c>
+      <c r="B55" s="5" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="56" ht="26" spans="1:2">
+      <c r="A56" s="4" t="s">
+        <v>402</v>
+      </c>
+      <c r="B56" s="5" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="57" ht="26" spans="1:2">
+      <c r="A57" s="4" t="s">
+        <v>403</v>
+      </c>
+      <c r="B57" s="5" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="58" ht="26" spans="1:2">
+      <c r="A58" s="4" t="s">
+        <v>404</v>
+      </c>
+      <c r="B58" s="5" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="59" ht="26" spans="1:2">
+      <c r="A59" s="4" t="s">
+        <v>405</v>
+      </c>
+      <c r="B59" s="5" t="s">
+        <v>155</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Test case updated til the Admin Functionality
</commit_message>
<xml_diff>
--- a/OrangeHRM_Test_Cases.xlsx
+++ b/OrangeHRM_Test_Cases.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="607" uniqueCount="406">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="621" uniqueCount="416">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -1765,10 +1765,53 @@
     <t>TC_AF_054</t>
   </si>
   <si>
+    <t xml:space="preserve">Validate the "Add Nationality" functionality with valid inputs
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. click on the 'Admin' button from the left sidebar.
+2. Click on Nationality&gt;"+Add"
+3.Input a valid nationlaity in the "Name" field. 
+4. Click on the 'Save' button. </t>
+  </si>
+  <si>
+    <t>*Name: Lebanese</t>
+  </si>
+  <si>
+    <t>1. System should add the nationality if not added previously.</t>
+  </si>
+  <si>
     <t>TC_AF_055</t>
   </si>
   <si>
+    <t xml:space="preserve">Validate the "Add Nationality" functionality with invalid inputs
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. click on the 'Admin' button from the left sidebar.
+2. Click on Nationality&gt;"+Add"
+3.Input a invalid nationlaity in the "Name" field. 
+4. Click on the 'Save' button. </t>
+  </si>
+  <si>
+    <t>*Name: hhg1247</t>
+  </si>
+  <si>
     <t>TC_AF_056</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Validate the "Add Nationality" functionality with empty fields. 
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. click on the 'Admin' button from the left sidebar.
+2. Click on Nationality&gt;"+Add"
+3.Input nothingin the "Name" field. 
+4. Click on the 'Save' button. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. System should ask for the inputs or pop up messege to input required fields.
+</t>
   </si>
   <si>
     <t>TC_AF_057</t>
@@ -31895,8 +31938,8 @@
   <sheetPr/>
   <dimension ref="A1:K59"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="87" zoomScaleNormal="87" topLeftCell="A54" workbookViewId="0">
-      <selection activeCell="E55" sqref="E55"/>
+    <sheetView tabSelected="1" zoomScale="87" zoomScaleNormal="87" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="D57" sqref="D57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5"/>
@@ -33133,33 +33176,75 @@
         <v>361</v>
       </c>
     </row>
-    <row r="55" ht="26" spans="1:2">
+    <row r="55" ht="145" spans="1:7">
       <c r="A55" s="4" t="s">
         <v>401</v>
       </c>
       <c r="B55" s="5" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="56" ht="26" spans="1:2">
+      <c r="C55" s="9" t="s">
+        <v>402</v>
+      </c>
+      <c r="D55" s="6" t="s">
+        <v>157</v>
+      </c>
+      <c r="E55" s="7" t="s">
+        <v>403</v>
+      </c>
+      <c r="F55" t="s">
+        <v>404</v>
+      </c>
+      <c r="G55" s="9" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="56" ht="145" spans="1:7">
       <c r="A56" s="4" t="s">
-        <v>402</v>
+        <v>406</v>
       </c>
       <c r="B56" s="5" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="57" ht="26" spans="1:2">
+      <c r="C56" s="9" t="s">
+        <v>407</v>
+      </c>
+      <c r="D56" s="6" t="s">
+        <v>157</v>
+      </c>
+      <c r="E56" s="7" t="s">
+        <v>408</v>
+      </c>
+      <c r="F56" t="s">
+        <v>409</v>
+      </c>
+      <c r="G56" s="9" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="57" ht="130.5" spans="1:7">
       <c r="A57" s="4" t="s">
-        <v>403</v>
+        <v>410</v>
       </c>
       <c r="B57" s="5" t="s">
         <v>155</v>
       </c>
+      <c r="C57" s="9" t="s">
+        <v>411</v>
+      </c>
+      <c r="D57" s="6" t="s">
+        <v>157</v>
+      </c>
+      <c r="E57" s="7" t="s">
+        <v>412</v>
+      </c>
+      <c r="G57" s="9" t="s">
+        <v>413</v>
+      </c>
     </row>
     <row r="58" ht="26" spans="1:2">
       <c r="A58" s="4" t="s">
-        <v>404</v>
+        <v>414</v>
       </c>
       <c r="B58" s="5" t="s">
         <v>155</v>
@@ -33167,7 +33252,7 @@
     </row>
     <row r="59" ht="26" spans="1:2">
       <c r="A59" s="4" t="s">
-        <v>405</v>
+        <v>415</v>
       </c>
       <c r="B59" s="5" t="s">
         <v>155</v>

</xml_diff>

<commit_message>
Deleted 2 extra rows
</commit_message>
<xml_diff>
--- a/OrangeHRM_Test_Cases.xlsx
+++ b/OrangeHRM_Test_Cases.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="621" uniqueCount="416">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="617" uniqueCount="414">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -1812,12 +1812,6 @@
   <si>
     <t xml:space="preserve">1. System should ask for the inputs or pop up messege to input required fields.
 </t>
-  </si>
-  <si>
-    <t>TC_AF_057</t>
-  </si>
-  <si>
-    <t>TC_AF_058</t>
   </si>
 </sst>
 </file>
@@ -3323,7 +3317,7 @@
   <sheetPr/>
   <dimension ref="A1:Z998"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" topLeftCell="A21" workbookViewId="0">
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
@@ -31616,7 +31610,7 @@
   <sheetPr/>
   <dimension ref="A1:K10"/>
   <sheetViews>
-    <sheetView zoomScale="64" zoomScaleNormal="64" workbookViewId="0">
+    <sheetView zoomScale="64" zoomScaleNormal="64" topLeftCell="A6" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -31938,8 +31932,8 @@
   <sheetPr/>
   <dimension ref="A1:K59"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="87" zoomScaleNormal="87" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="D57" sqref="D57"/>
+    <sheetView tabSelected="1" zoomScale="87" zoomScaleNormal="87" topLeftCell="A56" workbookViewId="0">
+      <selection activeCell="C63" sqref="C63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5"/>
@@ -33242,21 +33236,13 @@
         <v>413</v>
       </c>
     </row>
-    <row r="58" ht="26" spans="1:2">
-      <c r="A58" s="4" t="s">
-        <v>414</v>
-      </c>
-      <c r="B58" s="5" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="59" ht="26" spans="1:2">
-      <c r="A59" s="4" t="s">
-        <v>415</v>
-      </c>
-      <c r="B59" s="5" t="s">
-        <v>155</v>
-      </c>
+    <row r="58" spans="1:2">
+      <c r="A58" s="4"/>
+      <c r="B58" s="5"/>
+    </row>
+    <row r="59" spans="1:2">
+      <c r="A59" s="4"/>
+      <c r="B59" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Test case update done
</commit_message>
<xml_diff>
--- a/OrangeHRM_Test_Cases.xlsx
+++ b/OrangeHRM_Test_Cases.xlsx
@@ -4,13 +4,15 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19200" windowHeight="6200" activeTab="3"/>
+    <workbookView windowWidth="19200" windowHeight="6200" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Login" sheetId="1" r:id="rId1"/>
-    <sheet name="Logout" sheetId="2" r:id="rId2"/>
-    <sheet name="Admin" sheetId="3" r:id="rId3"/>
-    <sheet name="PIM" sheetId="4" r:id="rId4"/>
+    <sheet name="Project History" sheetId="5" r:id="rId1"/>
+    <sheet name="Test Scenario" sheetId="6" r:id="rId2"/>
+    <sheet name="Login" sheetId="1" r:id="rId3"/>
+    <sheet name="Logout" sheetId="2" r:id="rId4"/>
+    <sheet name="Admin" sheetId="3" r:id="rId5"/>
+    <sheet name="PIM" sheetId="4" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -30,7 +32,19 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="656" uniqueCount="433">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="667" uniqueCount="443">
+  <si>
+    <t>Project Name (Client Name)</t>
+  </si>
+  <si>
+    <t>OrangeHRM</t>
+  </si>
+  <si>
+    <t>Prepared By</t>
+  </si>
+  <si>
+    <t>Iqbal Shimul</t>
+  </si>
   <si>
     <t>Test Case ID</t>
   </si>
@@ -1825,7 +1839,7 @@
     <t>Validate the "Add Employee" Functionality with all valid inputs</t>
   </si>
   <si>
-    <t xml:space="preserve">1. Click on the "PIM" button form leftbar. 
+    <t>1. Click on the "PIM" button form leftbar. 
 2. Click on PIM&gt;"+Add" 
 3. Input a valid employee full name
 4. Input a valid Employee Id.
@@ -1834,7 +1848,7 @@
 7. Input a valid username
 8.Input a strong password for employee login.
 9. Confirm the password.
-3. Click on the search button. </t>
+10. Click on the save button.</t>
   </si>
   <si>
     <t xml:space="preserve">1. Employee details must create in the system.
@@ -1856,7 +1870,7 @@
 7. Input an invalid username
 8. Input a password for employee login.
 9. Confirm the password.
-3. Click on the search button. </t>
+10. Click on the save button. </t>
   </si>
   <si>
     <t>1. System will create the employee details with the input data.</t>
@@ -1865,34 +1879,73 @@
     <t>TC_PF_003</t>
   </si>
   <si>
-    <t>Validate the "Add Employee" Functionality with only input the employee name.</t>
+    <t>Validate the "Add Employee" Functionality with only filling the "Employee full name" field.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Click on the "PIM" button form leftbar. 
+2. Click on PIM&gt;"+Add"
+3. Input a valid employee full name.
+4. Input nothing in the "Employee Id" field. 
+5. Click on the save button. </t>
+  </si>
+  <si>
+    <t>1. System should ask for the employee id but will create the employee details.</t>
+  </si>
+  <si>
+    <t>TC_PF_004</t>
+  </si>
+  <si>
+    <t>Validate the "Add Employee" Functionality with only filling the valid "Employee Id" field.</t>
   </si>
   <si>
     <t xml:space="preserve">1. Click on the "PIM" button form leftbar. 
 2. Click on PIM&gt;"+Add" 
-3. Input a invalid employee full name
-4. Click on the search button. </t>
-  </si>
-  <si>
-    <t>1. System should ask for the employee id.</t>
-  </si>
-  <si>
-    <t>TC_PF_004</t>
+3.Input nothing in the "Employee Full Name" field.
+4. Input a valid employee ID.
+5. Click on the save button. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. System should ask for the Employee name. without employee name no action will happen in the system.
+</t>
   </si>
   <si>
     <t>TC_PF_005</t>
   </si>
   <si>
+    <t>Validate the "Add Employee" Functionality with all empty fields.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Click on the "PIM" button form leftbar. 
+2. Click on PIM&gt;"+Add" 
+3.Input nothing in the "Employee Full Name" field.
+3. Input nothing in the "Employee ID" field. 
+4. Click on the save button. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. System should ask for the inputs for the required fields.
+</t>
+  </si>
+  <si>
     <t>TC_PF_006</t>
   </si>
   <si>
-    <t>TC_PF_007</t>
-  </si>
-  <si>
-    <t>TC_PF_008</t>
-  </si>
-  <si>
-    <t>TC_PF_009</t>
+    <t xml:space="preserve">Validate the "Crete Login Details" Functionality with all emptt fields. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Click on the "PIM" button form leftbar. 
+2. Click on PIM&gt;"+Add" 
+3. Input nothing employee full name
+4. Input nothing Employee Id.
+5. Upload nothing in the image upload section
+6.  Enable "Create Login Details" function.
+7. Input nothin in the username.
+8. Input nothing in the password field.
+9. Input nothing in the confirm password field.
+10. Click on the save button. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. System should ask for the inputs for the required fields.
+</t>
   </si>
 </sst>
 </file>
@@ -2330,7 +2383,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="19">
+  <borders count="22">
     <border>
       <left/>
       <right/>
@@ -2482,6 +2535,51 @@
     </border>
     <border>
       <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
       <right style="thin">
@@ -2604,7 +2702,7 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="14" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -2616,34 +2714,34 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="8" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="8" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="8" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="8" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="9" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="9" borderId="19" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="21" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -2728,7 +2826,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -2843,6 +2941,17 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="6" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -3405,6 +3514,63 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
+  <dimension ref="E5:G6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="13" outlineLevelRow="5" outlineLevelCol="6"/>
+  <cols>
+    <col min="1" max="5" width="8.72727272727273" style="41"/>
+    <col min="6" max="6" width="49.8181818181818" style="41" customWidth="1"/>
+    <col min="7" max="7" width="27.1818181818182" style="41" customWidth="1"/>
+    <col min="8" max="16384" width="8.72727272727273" style="41"/>
+  </cols>
+  <sheetData>
+    <row r="5" ht="13.5" spans="5:7">
+      <c r="E5" s="42"/>
+      <c r="F5" s="43" t="s">
+        <v>0</v>
+      </c>
+      <c r="G5" s="44" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" ht="13.5" spans="5:7">
+      <c r="E6" s="45"/>
+      <c r="F6" s="46" t="s">
+        <v>2</v>
+      </c>
+      <c r="G6" s="47" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" topLeftCell="A21" workbookViewId="0">
@@ -3429,37 +3595,37 @@
   <sheetData>
     <row r="1" ht="15.25" spans="1:26">
       <c r="A1" s="23" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B1" s="24" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C1" s="25" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="D1" s="26" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="E1" s="26" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="F1" s="27" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="G1" s="26" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="H1" s="26" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="I1" s="26" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="J1" s="26" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="K1" s="40" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="L1" s="38"/>
       <c r="M1" s="38"/>
@@ -3479,25 +3645,25 @@
     </row>
     <row r="2" ht="203.25" spans="1:26">
       <c r="A2" s="28" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="B2" s="29" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="C2" s="30" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="D2" s="31" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="E2" s="32" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="F2" s="33" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="G2" s="32" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="H2" s="34"/>
       <c r="I2" s="34"/>
@@ -3521,25 +3687,25 @@
     </row>
     <row r="3" ht="189.75" spans="1:26">
       <c r="A3" s="28" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="B3" s="29" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="C3" s="30" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="D3" s="31" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="E3" s="32" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="F3" s="33" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="G3" s="32" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="H3" s="34"/>
       <c r="I3" s="34"/>
@@ -3563,25 +3729,25 @@
     </row>
     <row r="4" ht="189.75" spans="1:26">
       <c r="A4" s="28" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="B4" s="29" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="C4" s="30" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="D4" s="31" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="E4" s="32" t="s">
+        <v>31</v>
+      </c>
+      <c r="F4" s="33" t="s">
+        <v>32</v>
+      </c>
+      <c r="G4" s="32" t="s">
         <v>27</v>
-      </c>
-      <c r="F4" s="33" t="s">
-        <v>28</v>
-      </c>
-      <c r="G4" s="32" t="s">
-        <v>23</v>
       </c>
       <c r="H4" s="34"/>
       <c r="I4" s="34"/>
@@ -3605,25 +3771,25 @@
     </row>
     <row r="5" ht="189.75" spans="1:26">
       <c r="A5" s="28" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="B5" s="29" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="C5" s="30" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="D5" s="31" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="E5" s="32" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="F5" s="33" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="G5" s="32" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="H5" s="34"/>
       <c r="I5" s="34"/>
@@ -3647,25 +3813,25 @@
     </row>
     <row r="6" ht="162.75" spans="1:26">
       <c r="A6" s="28" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="B6" s="29" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="C6" s="30" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="D6" s="31" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="E6" s="32" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="F6" s="35" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="G6" s="32" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="H6" s="34"/>
       <c r="I6" s="34"/>
@@ -3689,25 +3855,25 @@
     </row>
     <row r="7" ht="108.75" spans="1:26">
       <c r="A7" s="28" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="B7" s="29" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="C7" s="30" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="D7" s="31" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="E7" s="32" t="s">
+        <v>46</v>
+      </c>
+      <c r="F7" s="35" t="s">
         <v>42</v>
       </c>
-      <c r="F7" s="35" t="s">
-        <v>38</v>
-      </c>
       <c r="G7" s="32" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="H7" s="34"/>
       <c r="I7" s="34"/>
@@ -3731,25 +3897,25 @@
     </row>
     <row r="8" ht="297.75" spans="1:26">
       <c r="A8" s="28" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="B8" s="29" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="C8" s="30" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="D8" s="31" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="E8" s="32" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="F8" s="35" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="G8" s="32" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="H8" s="36"/>
       <c r="I8" s="36"/>
@@ -3773,25 +3939,25 @@
     </row>
     <row r="9" ht="95.25" spans="1:26">
       <c r="A9" s="28" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="B9" s="29" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="C9" s="30" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="D9" s="31" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="E9" s="32" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="F9" s="35" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="G9" s="32" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="H9" s="34"/>
       <c r="I9" s="34"/>
@@ -3815,25 +3981,25 @@
     </row>
     <row r="10" ht="230.25" spans="1:26">
       <c r="A10" s="28" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="B10" s="29" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="C10" s="30" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="D10" s="31" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="E10" s="32" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="F10" s="33" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="G10" s="32" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="H10" s="34"/>
       <c r="I10" s="34"/>
@@ -3857,25 +4023,25 @@
     </row>
     <row r="11" ht="284.25" spans="1:26">
       <c r="A11" s="28" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B11" s="29" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="C11" s="30" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="D11" s="31" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="E11" s="32" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="F11" s="33" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="G11" s="32" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="H11" s="34"/>
       <c r="I11" s="34"/>
@@ -3899,25 +4065,25 @@
     </row>
     <row r="12" ht="216.75" spans="1:26">
       <c r="A12" s="28" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="B12" s="29" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="C12" s="30" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="D12" s="31" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="E12" s="32" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="F12" s="35" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="G12" s="32" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="H12" s="36"/>
       <c r="I12" s="34"/>
@@ -3941,25 +4107,25 @@
     </row>
     <row r="13" ht="230.25" spans="1:26">
       <c r="A13" s="28" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="B13" s="29" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="C13" s="30" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="D13" s="31" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="E13" s="32" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="F13" s="33" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="G13" s="32" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="H13" s="34"/>
       <c r="I13" s="34"/>
@@ -3983,25 +4149,25 @@
     </row>
     <row r="14" ht="122.25" spans="1:26">
       <c r="A14" s="28" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="B14" s="29" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="C14" s="30" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="D14" s="31" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="E14" s="32" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="F14" s="35" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="G14" s="32" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="H14" s="34"/>
       <c r="I14" s="34"/>
@@ -4025,25 +4191,25 @@
     </row>
     <row r="15" ht="216.75" spans="1:26">
       <c r="A15" s="28" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="B15" s="29" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="C15" s="30" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="D15" s="32" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="E15" s="32" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="F15" s="35" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="G15" s="32" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="H15" s="34"/>
       <c r="I15" s="34"/>
@@ -4067,25 +4233,25 @@
     </row>
     <row r="16" ht="176.25" spans="1:26">
       <c r="A16" s="28" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="B16" s="29" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="C16" s="30" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="D16" s="31" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="E16" s="32" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="F16" s="35" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="G16" s="32" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="H16" s="34"/>
       <c r="I16" s="34"/>
@@ -4109,25 +4275,25 @@
     </row>
     <row r="17" ht="409.5" spans="1:26">
       <c r="A17" s="28" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="B17" s="29" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="C17" s="30" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="D17" s="31" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="E17" s="32" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="F17" s="33" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="G17" s="32" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="H17" s="34"/>
       <c r="I17" s="34"/>
@@ -4151,25 +4317,25 @@
     </row>
     <row r="18" ht="257.25" spans="1:26">
       <c r="A18" s="28" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="B18" s="29" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="C18" s="30" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="D18" s="31" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="E18" s="32" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="F18" s="33" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="G18" s="32" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="H18" s="34"/>
       <c r="I18" s="34"/>
@@ -4193,25 +4359,25 @@
     </row>
     <row r="19" ht="270.75" spans="1:26">
       <c r="A19" s="28" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="B19" s="29" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="C19" s="30" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="D19" s="31" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="E19" s="32" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="F19" s="33" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="G19" s="32" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="H19" s="34"/>
       <c r="I19" s="34"/>
@@ -4235,25 +4401,25 @@
     </row>
     <row r="20" ht="216.75" spans="1:26">
       <c r="A20" s="28" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="B20" s="29" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="C20" s="30" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="D20" s="31" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="E20" s="32" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="F20" s="35" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="G20" s="32" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="H20" s="34"/>
       <c r="I20" s="34"/>
@@ -4277,25 +4443,25 @@
     </row>
     <row r="21" ht="203.25" spans="1:26">
       <c r="A21" s="28" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="B21" s="29" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="C21" s="30" t="s">
+        <v>115</v>
+      </c>
+      <c r="D21" s="31" t="s">
         <v>111</v>
       </c>
-      <c r="D21" s="31" t="s">
-        <v>107</v>
-      </c>
       <c r="E21" s="32" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="F21" s="35" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="G21" s="32" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="H21" s="34"/>
       <c r="I21" s="34"/>
@@ -4319,25 +4485,25 @@
     </row>
     <row r="22" ht="68.25" spans="1:26">
       <c r="A22" s="28" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="B22" s="29" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="C22" s="30" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="D22" s="31" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="E22" s="32" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="F22" s="35" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="G22" s="32" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="H22" s="34"/>
       <c r="I22" s="34"/>
@@ -31695,7 +31861,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
   <dimension ref="A1:K10"/>
@@ -31722,42 +31888,42 @@
   <sheetData>
     <row r="1" s="13" customFormat="1" spans="1:11">
       <c r="A1" s="3" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" s="14" customFormat="1" ht="12.75" customHeight="1" spans="1:11">
       <c r="A2" s="15" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="B2" s="15"/>
       <c r="C2" s="16"/>
@@ -31772,25 +31938,25 @@
     </row>
     <row r="3" s="13" customFormat="1" ht="109.5" customHeight="1" spans="1:11">
       <c r="A3" s="17" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="B3" s="18" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="C3" s="19" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="D3" s="19" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="E3" s="19" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="F3" s="18" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="G3" s="19" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="H3" s="20"/>
       <c r="I3" s="17"/>
@@ -31799,25 +31965,25 @@
     </row>
     <row r="4" s="13" customFormat="1" ht="54" spans="1:11">
       <c r="A4" s="17" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="B4" s="18" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="C4" s="19" t="s">
+        <v>130</v>
+      </c>
+      <c r="D4" s="19" t="s">
         <v>126</v>
       </c>
-      <c r="D4" s="19" t="s">
-        <v>122</v>
-      </c>
       <c r="E4" s="19" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="F4" s="18" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="G4" s="19" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
       <c r="H4" s="20"/>
       <c r="I4" s="20"/>
@@ -31826,25 +31992,25 @@
     </row>
     <row r="5" s="13" customFormat="1" ht="40.5" spans="1:11">
       <c r="A5" s="17" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
       <c r="B5" s="18" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="C5" s="19" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="D5" s="19" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="E5" s="19" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="F5" s="18" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="G5" s="19" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="H5" s="20"/>
       <c r="I5" s="20"/>
@@ -31853,25 +32019,25 @@
     </row>
     <row r="6" s="13" customFormat="1" ht="94.5" spans="1:11">
       <c r="A6" s="17" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="B6" s="18" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="C6" s="19" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
       <c r="D6" s="19" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="E6" s="19" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="F6" s="18" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="G6" s="19" t="s">
-        <v>137</v>
+        <v>141</v>
       </c>
       <c r="H6" s="20"/>
       <c r="I6" s="20"/>
@@ -31880,25 +32046,25 @@
     </row>
     <row r="7" s="13" customFormat="1" ht="54" spans="1:11">
       <c r="A7" s="17" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
       <c r="B7" s="18" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="C7" s="19" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="D7" s="19" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="E7" s="19" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="F7" s="18" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="G7" s="19" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="H7" s="20"/>
       <c r="I7" s="20"/>
@@ -31907,25 +32073,25 @@
     </row>
     <row r="8" s="13" customFormat="1" ht="67.5" spans="1:11">
       <c r="A8" s="17" t="s">
-        <v>142</v>
+        <v>146</v>
       </c>
       <c r="B8" s="18" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="C8" s="19" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="D8" s="19" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="E8" s="19" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
       <c r="F8" s="18" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="G8" s="19" t="s">
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="H8" s="20"/>
       <c r="I8" s="20"/>
@@ -31934,25 +32100,25 @@
     </row>
     <row r="9" s="13" customFormat="1" ht="54" spans="1:11">
       <c r="A9" s="17" t="s">
-        <v>147</v>
+        <v>151</v>
       </c>
       <c r="B9" s="18" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="C9" s="19" t="s">
+        <v>152</v>
+      </c>
+      <c r="D9" s="19" t="s">
         <v>148</v>
       </c>
-      <c r="D9" s="19" t="s">
-        <v>144</v>
-      </c>
       <c r="E9" s="19" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
       <c r="F9" s="17" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="G9" s="19" t="s">
-        <v>150</v>
+        <v>154</v>
       </c>
       <c r="H9" s="20"/>
       <c r="I9" s="20"/>
@@ -31961,25 +32127,25 @@
     </row>
     <row r="10" s="13" customFormat="1" ht="40.5" spans="1:11">
       <c r="A10" s="17" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
       <c r="B10" s="18" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="C10" s="19" t="s">
-        <v>152</v>
+        <v>156</v>
       </c>
       <c r="D10" s="19" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="E10" s="19" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
       <c r="F10" s="17" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="G10" s="19" t="s">
-        <v>153</v>
+        <v>157</v>
       </c>
       <c r="H10" s="20"/>
       <c r="I10" s="20"/>
@@ -32017,7 +32183,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
   <dimension ref="A1:K59"/>
@@ -32040,1288 +32206,1288 @@
   <sheetData>
     <row r="1" s="1" customFormat="1" ht="13.5" spans="1:11">
       <c r="A1" s="3" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" s="8" customFormat="1" ht="143" spans="1:7">
       <c r="A2" s="9" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>156</v>
+        <v>160</v>
       </c>
       <c r="D2"/>
       <c r="E2" s="6" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>158</v>
+        <v>162</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
     </row>
     <row r="3" ht="156" spans="1:7">
       <c r="A3" s="9" t="s">
-        <v>160</v>
+        <v>164</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>163</v>
+        <v>167</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>164</v>
+        <v>168</v>
       </c>
       <c r="G3" s="11" t="s">
-        <v>165</v>
+        <v>169</v>
       </c>
     </row>
     <row r="4" ht="156" spans="1:7">
       <c r="A4" s="9" t="s">
+        <v>170</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>159</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>171</v>
+      </c>
+      <c r="D4" s="6" t="s">
         <v>166</v>
       </c>
-      <c r="B4" s="10" t="s">
-        <v>155</v>
-      </c>
-      <c r="C4" s="11" t="s">
-        <v>167</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>162</v>
-      </c>
       <c r="E4" s="6" t="s">
-        <v>168</v>
+        <v>172</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
       <c r="G4" s="11" t="s">
-        <v>170</v>
+        <v>174</v>
       </c>
     </row>
     <row r="5" ht="156" spans="1:7">
       <c r="A5" s="9" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>173</v>
+        <v>177</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>174</v>
+        <v>178</v>
       </c>
       <c r="G5" s="11" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
     </row>
     <row r="6" ht="143" spans="1:7">
       <c r="A6" s="9" t="s">
-        <v>176</v>
+        <v>180</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>177</v>
+        <v>181</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>178</v>
+        <v>182</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>179</v>
+        <v>183</v>
       </c>
       <c r="G6" s="11" t="s">
-        <v>170</v>
+        <v>174</v>
       </c>
     </row>
     <row r="7" ht="143" spans="1:7">
       <c r="A7" s="9" t="s">
-        <v>180</v>
+        <v>184</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>183</v>
+        <v>187</v>
       </c>
       <c r="G7" s="11" t="s">
-        <v>184</v>
+        <v>188</v>
       </c>
     </row>
     <row r="8" ht="143" spans="1:7">
       <c r="A8" s="9" t="s">
-        <v>185</v>
+        <v>189</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>186</v>
+        <v>190</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>188</v>
+        <v>192</v>
       </c>
       <c r="G8" s="11" t="s">
-        <v>189</v>
+        <v>193</v>
       </c>
     </row>
     <row r="9" ht="156" spans="1:7">
       <c r="A9" s="9" t="s">
-        <v>190</v>
+        <v>194</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>191</v>
+        <v>195</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>192</v>
+        <v>196</v>
       </c>
       <c r="F9" s="12" t="s">
-        <v>193</v>
+        <v>197</v>
       </c>
       <c r="G9" s="11" t="s">
-        <v>194</v>
+        <v>198</v>
       </c>
     </row>
     <row r="10" ht="232" spans="1:7">
       <c r="A10" s="9" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>196</v>
+        <v>200</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="E10" s="11" t="s">
-        <v>197</v>
+        <v>201</v>
       </c>
       <c r="F10" s="11" t="s">
-        <v>198</v>
+        <v>202</v>
       </c>
       <c r="G10" s="11" t="s">
-        <v>199</v>
+        <v>203</v>
       </c>
     </row>
     <row r="11" ht="261" spans="1:7">
       <c r="A11" s="9" t="s">
-        <v>200</v>
+        <v>204</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="E11" s="11" t="s">
-        <v>202</v>
+        <v>206</v>
       </c>
       <c r="F11" s="11" t="s">
-        <v>203</v>
+        <v>207</v>
       </c>
       <c r="G11" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
     </row>
     <row r="12" ht="232" spans="1:7">
       <c r="A12" s="9" t="s">
-        <v>205</v>
+        <v>209</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>206</v>
+        <v>210</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="E12" s="11" t="s">
-        <v>207</v>
+        <v>211</v>
       </c>
       <c r="F12" s="11" t="s">
-        <v>208</v>
+        <v>212</v>
       </c>
       <c r="G12" s="11" t="s">
-        <v>209</v>
+        <v>213</v>
       </c>
     </row>
     <row r="13" ht="246.5" spans="1:7">
       <c r="A13" s="9" t="s">
-        <v>210</v>
+        <v>214</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>211</v>
+        <v>215</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="E13" s="11" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
       <c r="F13" s="11" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="G13" s="11" t="s">
-        <v>214</v>
+        <v>218</v>
       </c>
     </row>
     <row r="14" ht="232" spans="1:7">
       <c r="A14" s="9" t="s">
-        <v>215</v>
+        <v>219</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>216</v>
+        <v>220</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="E14" s="11" t="s">
-        <v>217</v>
+        <v>221</v>
       </c>
       <c r="F14" s="11" t="s">
-        <v>218</v>
+        <v>222</v>
       </c>
       <c r="G14" s="11" t="s">
-        <v>219</v>
+        <v>223</v>
       </c>
     </row>
     <row r="15" ht="232" spans="1:7">
       <c r="A15" s="9" t="s">
-        <v>220</v>
+        <v>224</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>221</v>
+        <v>225</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="E15" s="11" t="s">
-        <v>222</v>
+        <v>226</v>
       </c>
       <c r="F15" s="11" t="s">
-        <v>223</v>
+        <v>227</v>
       </c>
       <c r="G15" s="11" t="s">
-        <v>224</v>
+        <v>228</v>
       </c>
     </row>
     <row r="16" ht="232" spans="1:7">
       <c r="A16" s="9" t="s">
-        <v>225</v>
+        <v>229</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>226</v>
+        <v>230</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="E16" s="11" t="s">
-        <v>227</v>
+        <v>231</v>
       </c>
       <c r="G16" s="11" t="s">
-        <v>228</v>
+        <v>232</v>
       </c>
     </row>
     <row r="17" ht="130.5" spans="1:7">
       <c r="A17" s="9" t="s">
-        <v>229</v>
+        <v>233</v>
       </c>
       <c r="B17" s="10" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="C17" s="11" t="s">
-        <v>230</v>
+        <v>234</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="E17" s="11" t="s">
-        <v>231</v>
+        <v>235</v>
       </c>
       <c r="F17" t="s">
-        <v>232</v>
+        <v>236</v>
       </c>
       <c r="G17" s="11" t="s">
-        <v>233</v>
+        <v>237</v>
       </c>
     </row>
     <row r="18" ht="130.5" spans="1:7">
       <c r="A18" s="9" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="C18" s="11" t="s">
-        <v>235</v>
+        <v>239</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="E18" s="11" t="s">
-        <v>236</v>
+        <v>240</v>
       </c>
       <c r="F18" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="G18" s="11" t="s">
-        <v>238</v>
+        <v>242</v>
       </c>
     </row>
     <row r="19" ht="145" spans="1:7">
       <c r="A19" s="9" t="s">
-        <v>239</v>
+        <v>243</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="C19" s="11" t="s">
-        <v>240</v>
+        <v>244</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="E19" s="11" t="s">
-        <v>241</v>
+        <v>245</v>
       </c>
       <c r="F19" t="s">
-        <v>242</v>
+        <v>246</v>
       </c>
       <c r="G19" s="11" t="s">
-        <v>243</v>
+        <v>247</v>
       </c>
     </row>
     <row r="20" ht="130.5" spans="1:7">
       <c r="A20" s="9" t="s">
-        <v>244</v>
+        <v>248</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="C20" s="11" t="s">
-        <v>245</v>
+        <v>249</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="E20" s="11" t="s">
-        <v>246</v>
+        <v>250</v>
       </c>
       <c r="F20" t="s">
-        <v>193</v>
+        <v>197</v>
       </c>
       <c r="G20" s="11" t="s">
-        <v>247</v>
+        <v>251</v>
       </c>
     </row>
     <row r="21" ht="145" spans="1:7">
       <c r="A21" s="9" t="s">
-        <v>248</v>
+        <v>252</v>
       </c>
       <c r="B21" s="10" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="C21" s="11" t="s">
-        <v>249</v>
+        <v>253</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="E21" s="11" t="s">
-        <v>250</v>
+        <v>254</v>
       </c>
       <c r="F21" t="s">
-        <v>251</v>
+        <v>255</v>
       </c>
       <c r="G21" s="11" t="s">
-        <v>252</v>
+        <v>256</v>
       </c>
     </row>
     <row r="22" ht="145" spans="1:7">
       <c r="A22" s="9" t="s">
-        <v>253</v>
+        <v>257</v>
       </c>
       <c r="B22" s="10" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="C22" s="11" t="s">
-        <v>254</v>
+        <v>258</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="E22" s="11" t="s">
-        <v>255</v>
+        <v>259</v>
       </c>
       <c r="F22" t="s">
-        <v>256</v>
+        <v>260</v>
       </c>
       <c r="G22" s="11" t="s">
-        <v>257</v>
+        <v>261</v>
       </c>
     </row>
     <row r="23" ht="145" spans="1:7">
       <c r="A23" s="9" t="s">
-        <v>258</v>
+        <v>262</v>
       </c>
       <c r="B23" s="10" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="C23" s="11" t="s">
-        <v>259</v>
+        <v>263</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="E23" s="11" t="s">
-        <v>260</v>
+        <v>264</v>
       </c>
       <c r="F23" t="s">
-        <v>261</v>
+        <v>265</v>
       </c>
       <c r="G23" s="11" t="s">
-        <v>262</v>
+        <v>266</v>
       </c>
     </row>
     <row r="24" ht="145" spans="1:7">
       <c r="A24" s="9" t="s">
-        <v>263</v>
+        <v>267</v>
       </c>
       <c r="B24" s="10" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="C24" s="11" t="s">
-        <v>264</v>
+        <v>268</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="E24" s="11" t="s">
-        <v>265</v>
+        <v>269</v>
       </c>
       <c r="F24" t="s">
-        <v>193</v>
+        <v>197</v>
       </c>
       <c r="G24" s="11" t="s">
-        <v>247</v>
+        <v>251</v>
       </c>
     </row>
     <row r="25" ht="130.5" spans="1:7">
       <c r="A25" s="9" t="s">
-        <v>266</v>
+        <v>270</v>
       </c>
       <c r="B25" s="10" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="C25" s="11" t="s">
-        <v>267</v>
+        <v>271</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="E25" s="11" t="s">
-        <v>268</v>
+        <v>272</v>
       </c>
       <c r="F25" s="11" t="s">
-        <v>269</v>
+        <v>273</v>
       </c>
       <c r="G25" s="11" t="s">
-        <v>270</v>
+        <v>274</v>
       </c>
     </row>
     <row r="26" ht="130.5" spans="1:7">
       <c r="A26" s="9" t="s">
-        <v>271</v>
+        <v>275</v>
       </c>
       <c r="B26" s="10" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="C26" s="11" t="s">
-        <v>272</v>
+        <v>276</v>
       </c>
       <c r="D26" s="6" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="E26" s="11" t="s">
-        <v>273</v>
+        <v>277</v>
       </c>
       <c r="F26" s="11" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="G26" s="11" t="s">
-        <v>275</v>
+        <v>279</v>
       </c>
     </row>
     <row r="27" ht="145" spans="1:7">
       <c r="A27" s="9" t="s">
-        <v>276</v>
+        <v>280</v>
       </c>
       <c r="B27" s="10" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="C27" s="11" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="D27" s="6" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="E27" s="11" t="s">
-        <v>278</v>
+        <v>282</v>
       </c>
       <c r="F27" t="s">
-        <v>242</v>
+        <v>246</v>
       </c>
       <c r="G27" s="11" t="s">
-        <v>279</v>
+        <v>283</v>
       </c>
     </row>
     <row r="28" ht="145" spans="1:7">
       <c r="A28" s="9" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="B28" s="10" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="C28" s="11" t="s">
-        <v>281</v>
+        <v>285</v>
       </c>
       <c r="D28" s="6" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="E28" s="11" t="s">
-        <v>282</v>
+        <v>286</v>
       </c>
       <c r="F28" t="s">
-        <v>193</v>
+        <v>197</v>
       </c>
       <c r="G28" s="11" t="s">
-        <v>283</v>
+        <v>287</v>
       </c>
     </row>
     <row r="29" ht="232" spans="1:7">
       <c r="A29" s="9" t="s">
-        <v>284</v>
+        <v>288</v>
       </c>
       <c r="B29" s="10" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="C29" s="11" t="s">
-        <v>285</v>
+        <v>289</v>
       </c>
       <c r="D29" s="6" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="E29" s="11" t="s">
-        <v>286</v>
+        <v>290</v>
       </c>
       <c r="F29" s="11" t="s">
-        <v>287</v>
+        <v>291</v>
       </c>
       <c r="G29" s="11" t="s">
-        <v>288</v>
+        <v>292</v>
       </c>
     </row>
     <row r="30" ht="232" spans="1:7">
       <c r="A30" s="9" t="s">
-        <v>289</v>
+        <v>293</v>
       </c>
       <c r="B30" s="10" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="C30" s="11" t="s">
-        <v>290</v>
+        <v>294</v>
       </c>
       <c r="D30" s="6" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="E30" s="11" t="s">
-        <v>291</v>
+        <v>295</v>
       </c>
       <c r="F30" s="11" t="s">
-        <v>292</v>
+        <v>296</v>
       </c>
       <c r="G30" s="11" t="s">
-        <v>293</v>
+        <v>297</v>
       </c>
     </row>
     <row r="31" ht="246.5" spans="1:7">
       <c r="A31" s="9" t="s">
-        <v>294</v>
+        <v>298</v>
       </c>
       <c r="B31" s="10" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="C31" s="11" t="s">
-        <v>295</v>
+        <v>299</v>
       </c>
       <c r="D31" s="6" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="E31" s="11" t="s">
-        <v>296</v>
+        <v>300</v>
       </c>
       <c r="F31" s="11" t="s">
-        <v>297</v>
+        <v>301</v>
       </c>
       <c r="G31" s="11" t="s">
-        <v>298</v>
+        <v>302</v>
       </c>
     </row>
     <row r="32" ht="246.5" spans="1:7">
       <c r="A32" s="9" t="s">
-        <v>299</v>
+        <v>303</v>
       </c>
       <c r="B32" s="10" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="C32" s="11" t="s">
-        <v>300</v>
+        <v>304</v>
       </c>
       <c r="D32" s="6" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="E32" s="11" t="s">
-        <v>301</v>
+        <v>305</v>
       </c>
       <c r="F32" s="11" t="s">
-        <v>302</v>
+        <v>306</v>
       </c>
       <c r="G32" s="11" t="s">
-        <v>303</v>
+        <v>307</v>
       </c>
     </row>
     <row r="33" ht="246.5" spans="1:7">
       <c r="A33" s="9" t="s">
-        <v>304</v>
+        <v>308</v>
       </c>
       <c r="B33" s="10" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="C33" s="11" t="s">
-        <v>305</v>
+        <v>309</v>
       </c>
       <c r="D33" s="6" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="E33" s="11" t="s">
-        <v>306</v>
+        <v>310</v>
       </c>
       <c r="F33" t="s">
-        <v>193</v>
+        <v>197</v>
       </c>
       <c r="G33" s="11" t="s">
-        <v>307</v>
+        <v>311</v>
       </c>
     </row>
     <row r="34" ht="409.5" spans="1:7">
       <c r="A34" s="9" t="s">
-        <v>308</v>
+        <v>312</v>
       </c>
       <c r="B34" s="10" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="C34" s="11" t="s">
-        <v>309</v>
+        <v>313</v>
       </c>
       <c r="D34" s="6" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="E34" s="11" t="s">
-        <v>310</v>
+        <v>314</v>
       </c>
       <c r="G34" s="11" t="s">
-        <v>311</v>
+        <v>315</v>
       </c>
     </row>
     <row r="35" ht="409.5" spans="1:7">
       <c r="A35" s="9" t="s">
-        <v>312</v>
+        <v>316</v>
       </c>
       <c r="B35" s="10" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="C35" s="11" t="s">
-        <v>313</v>
+        <v>317</v>
       </c>
       <c r="D35" s="6" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="E35" s="11" t="s">
-        <v>314</v>
+        <v>318</v>
       </c>
       <c r="G35" s="11" t="s">
-        <v>315</v>
+        <v>319</v>
       </c>
     </row>
     <row r="36" ht="409.5" spans="1:7">
       <c r="A36" s="9" t="s">
-        <v>316</v>
+        <v>320</v>
       </c>
       <c r="B36" s="10" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="C36" s="11" t="s">
-        <v>317</v>
+        <v>321</v>
       </c>
       <c r="D36" s="6" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="E36" s="11" t="s">
-        <v>318</v>
+        <v>322</v>
       </c>
       <c r="G36" s="11" t="s">
-        <v>319</v>
+        <v>323</v>
       </c>
     </row>
     <row r="37" ht="409.5" spans="1:7">
       <c r="A37" s="9" t="s">
-        <v>320</v>
+        <v>324</v>
       </c>
       <c r="B37" s="10" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="C37" s="11" t="s">
-        <v>321</v>
+        <v>325</v>
       </c>
       <c r="E37" s="11" t="s">
-        <v>322</v>
+        <v>326</v>
       </c>
       <c r="G37" s="11" t="s">
-        <v>323</v>
+        <v>327</v>
       </c>
     </row>
     <row r="38" ht="203" spans="1:7">
       <c r="A38" s="9" t="s">
-        <v>324</v>
+        <v>328</v>
       </c>
       <c r="B38" s="10" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="C38" s="11" t="s">
-        <v>325</v>
+        <v>329</v>
       </c>
       <c r="D38" s="6" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="E38" s="11" t="s">
-        <v>326</v>
+        <v>330</v>
       </c>
       <c r="F38" s="11" t="s">
-        <v>327</v>
+        <v>331</v>
       </c>
       <c r="G38" t="s">
-        <v>328</v>
+        <v>332</v>
       </c>
     </row>
     <row r="39" ht="203" spans="1:7">
       <c r="A39" s="9" t="s">
-        <v>329</v>
+        <v>333</v>
       </c>
       <c r="B39" s="10" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="C39" s="11" t="s">
-        <v>330</v>
+        <v>334</v>
       </c>
       <c r="D39" s="6" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="E39" s="11" t="s">
-        <v>331</v>
+        <v>335</v>
       </c>
       <c r="F39" s="11" t="s">
-        <v>332</v>
+        <v>336</v>
       </c>
       <c r="G39" s="11" t="s">
-        <v>333</v>
+        <v>337</v>
       </c>
     </row>
     <row r="40" ht="188.5" spans="1:7">
       <c r="A40" s="9" t="s">
-        <v>334</v>
+        <v>338</v>
       </c>
       <c r="B40" s="10" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="C40" s="11" t="s">
-        <v>335</v>
+        <v>339</v>
       </c>
       <c r="D40" s="6" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="E40" s="11" t="s">
-        <v>336</v>
+        <v>340</v>
       </c>
       <c r="F40" s="11" t="s">
-        <v>337</v>
+        <v>341</v>
       </c>
       <c r="G40" s="11" t="s">
-        <v>338</v>
+        <v>342</v>
       </c>
     </row>
     <row r="41" ht="188.5" spans="1:7">
       <c r="A41" s="9" t="s">
-        <v>339</v>
+        <v>343</v>
       </c>
       <c r="B41" s="10" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="C41" s="11" t="s">
-        <v>340</v>
+        <v>344</v>
       </c>
       <c r="D41" s="6" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="E41" s="11" t="s">
-        <v>341</v>
+        <v>345</v>
       </c>
       <c r="F41" t="s">
-        <v>342</v>
+        <v>346</v>
       </c>
       <c r="G41" s="11" t="s">
-        <v>343</v>
+        <v>347</v>
       </c>
     </row>
     <row r="42" ht="174" spans="1:7">
       <c r="A42" s="9" t="s">
-        <v>344</v>
+        <v>348</v>
       </c>
       <c r="B42" s="10" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="C42" s="11" t="s">
-        <v>345</v>
+        <v>349</v>
       </c>
       <c r="D42" s="6" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="E42" s="11" t="s">
-        <v>346</v>
+        <v>350</v>
       </c>
       <c r="G42" s="11" t="s">
-        <v>347</v>
+        <v>351</v>
       </c>
     </row>
     <row r="43" ht="159.5" spans="1:7">
       <c r="A43" s="9" t="s">
-        <v>348</v>
+        <v>352</v>
       </c>
       <c r="B43" s="10" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="C43" s="11" t="s">
-        <v>349</v>
+        <v>353</v>
       </c>
       <c r="D43" s="6" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="E43" s="11" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F43" t="s">
-        <v>351</v>
+        <v>355</v>
       </c>
       <c r="G43" s="11" t="s">
-        <v>352</v>
+        <v>356</v>
       </c>
     </row>
     <row r="44" ht="174" spans="1:7">
       <c r="A44" s="9" t="s">
-        <v>353</v>
+        <v>357</v>
       </c>
       <c r="B44" s="10" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="C44" s="11" t="s">
-        <v>354</v>
+        <v>358</v>
       </c>
       <c r="D44" s="6" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="E44" s="11" t="s">
-        <v>355</v>
+        <v>359</v>
       </c>
       <c r="F44" t="s">
-        <v>356</v>
+        <v>360</v>
       </c>
       <c r="G44" s="11" t="s">
-        <v>357</v>
+        <v>361</v>
       </c>
     </row>
     <row r="45" ht="145" spans="1:7">
       <c r="A45" s="9" t="s">
-        <v>358</v>
+        <v>362</v>
       </c>
       <c r="B45" s="10" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="C45" s="11" t="s">
-        <v>359</v>
+        <v>363</v>
       </c>
       <c r="D45" s="6" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="E45" s="11" t="s">
-        <v>360</v>
+        <v>364</v>
       </c>
       <c r="G45" s="11" t="s">
-        <v>361</v>
+        <v>365</v>
       </c>
     </row>
     <row r="46" ht="159.5" spans="1:8">
       <c r="A46" s="9" t="s">
-        <v>362</v>
+        <v>366</v>
       </c>
       <c r="B46" s="10" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="C46" s="11" t="s">
-        <v>363</v>
+        <v>367</v>
       </c>
       <c r="D46" s="6" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="E46" s="11" t="s">
-        <v>364</v>
+        <v>368</v>
       </c>
       <c r="F46" s="11" t="s">
-        <v>365</v>
+        <v>369</v>
       </c>
       <c r="G46" s="11" t="s">
-        <v>366</v>
+        <v>370</v>
       </c>
       <c r="H46" s="11"/>
     </row>
     <row r="47" ht="159.5" spans="1:7">
       <c r="A47" s="9" t="s">
-        <v>367</v>
+        <v>371</v>
       </c>
       <c r="B47" s="10" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="C47" s="11" t="s">
-        <v>368</v>
+        <v>372</v>
       </c>
       <c r="D47" s="6" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="E47" s="11" t="s">
-        <v>369</v>
+        <v>373</v>
       </c>
       <c r="F47" s="11" t="s">
-        <v>370</v>
+        <v>374</v>
       </c>
       <c r="G47" s="11" t="s">
-        <v>371</v>
+        <v>375</v>
       </c>
     </row>
     <row r="48" ht="145" spans="1:7">
       <c r="A48" s="9" t="s">
-        <v>372</v>
+        <v>376</v>
       </c>
       <c r="B48" s="10" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="C48" s="11" t="s">
-        <v>373</v>
+        <v>377</v>
       </c>
       <c r="D48" s="6" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="E48" s="11" t="s">
-        <v>374</v>
+        <v>378</v>
       </c>
       <c r="G48" s="11" t="s">
-        <v>361</v>
+        <v>365</v>
       </c>
     </row>
     <row r="49" ht="159.5" spans="1:7">
       <c r="A49" s="9" t="s">
-        <v>375</v>
+        <v>379</v>
       </c>
       <c r="B49" s="10" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="C49" s="11" t="s">
-        <v>376</v>
+        <v>380</v>
       </c>
       <c r="D49" s="6" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="E49" s="11" t="s">
-        <v>377</v>
+        <v>381</v>
       </c>
       <c r="F49" t="s">
-        <v>378</v>
+        <v>382</v>
       </c>
       <c r="G49" s="11" t="s">
-        <v>379</v>
+        <v>383</v>
       </c>
     </row>
     <row r="50" ht="159.5" spans="1:7">
       <c r="A50" s="9" t="s">
-        <v>380</v>
+        <v>384</v>
       </c>
       <c r="B50" s="10" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="C50" s="11" t="s">
-        <v>381</v>
+        <v>385</v>
       </c>
       <c r="D50" s="6" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="E50" s="11" t="s">
-        <v>382</v>
+        <v>386</v>
       </c>
       <c r="F50" t="s">
-        <v>383</v>
+        <v>387</v>
       </c>
       <c r="G50" t="s">
-        <v>384</v>
+        <v>388</v>
       </c>
     </row>
     <row r="51" ht="145" spans="1:7">
       <c r="A51" s="9" t="s">
-        <v>385</v>
+        <v>389</v>
       </c>
       <c r="B51" s="10" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="C51" s="11" t="s">
-        <v>386</v>
+        <v>390</v>
       </c>
       <c r="D51" s="6" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="E51" s="11" t="s">
-        <v>387</v>
+        <v>391</v>
       </c>
       <c r="G51" s="11" t="s">
-        <v>388</v>
+        <v>392</v>
       </c>
     </row>
     <row r="52" ht="159.5" spans="1:7">
       <c r="A52" s="9" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
       <c r="B52" s="10" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="C52" s="11" t="s">
-        <v>390</v>
+        <v>394</v>
       </c>
       <c r="D52" s="6" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="E52" s="11" t="s">
-        <v>391</v>
+        <v>395</v>
       </c>
       <c r="F52" t="s">
-        <v>392</v>
+        <v>396</v>
       </c>
       <c r="G52" s="11" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
     </row>
     <row r="53" ht="159.5" spans="1:7">
       <c r="A53" s="9" t="s">
-        <v>394</v>
+        <v>398</v>
       </c>
       <c r="B53" s="10" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="C53" s="11" t="s">
-        <v>395</v>
+        <v>399</v>
       </c>
       <c r="D53" s="6" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="E53" s="11" t="s">
-        <v>396</v>
+        <v>400</v>
       </c>
       <c r="F53" t="s">
+        <v>401</v>
+      </c>
+      <c r="G53" s="11" t="s">
         <v>397</v>
-      </c>
-      <c r="G53" s="11" t="s">
-        <v>393</v>
       </c>
     </row>
     <row r="54" ht="145" spans="1:7">
       <c r="A54" s="9" t="s">
-        <v>398</v>
+        <v>402</v>
       </c>
       <c r="B54" s="10" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="C54" s="11" t="s">
-        <v>399</v>
+        <v>403</v>
       </c>
       <c r="D54" s="6" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="E54" s="11" t="s">
-        <v>400</v>
+        <v>404</v>
       </c>
       <c r="G54" s="11" t="s">
-        <v>361</v>
+        <v>365</v>
       </c>
     </row>
     <row r="55" ht="145" spans="1:7">
       <c r="A55" s="9" t="s">
-        <v>401</v>
+        <v>405</v>
       </c>
       <c r="B55" s="10" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="C55" s="11" t="s">
-        <v>402</v>
+        <v>406</v>
       </c>
       <c r="D55" s="6" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="E55" s="11" t="s">
-        <v>403</v>
+        <v>407</v>
       </c>
       <c r="F55" t="s">
-        <v>404</v>
+        <v>408</v>
       </c>
       <c r="G55" s="11" t="s">
-        <v>405</v>
+        <v>409</v>
       </c>
     </row>
     <row r="56" ht="145" spans="1:7">
       <c r="A56" s="9" t="s">
-        <v>406</v>
+        <v>410</v>
       </c>
       <c r="B56" s="10" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="C56" s="11" t="s">
-        <v>407</v>
+        <v>411</v>
       </c>
       <c r="D56" s="6" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="E56" s="11" t="s">
-        <v>408</v>
+        <v>412</v>
       </c>
       <c r="F56" t="s">
+        <v>413</v>
+      </c>
+      <c r="G56" s="11" t="s">
         <v>409</v>
-      </c>
-      <c r="G56" s="11" t="s">
-        <v>405</v>
       </c>
     </row>
     <row r="57" ht="130.5" spans="1:7">
       <c r="A57" s="9" t="s">
-        <v>410</v>
+        <v>414</v>
       </c>
       <c r="B57" s="10" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="C57" s="11" t="s">
-        <v>411</v>
+        <v>415</v>
       </c>
       <c r="D57" s="6" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="E57" s="11" t="s">
-        <v>412</v>
+        <v>416</v>
       </c>
       <c r="G57" s="11" t="s">
-        <v>413</v>
+        <v>417</v>
       </c>
     </row>
     <row r="58" spans="1:2">
@@ -33338,13 +33504,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:K10"/>
+  <dimension ref="A1:K9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5"/>
@@ -33361,143 +33527,164 @@
   <sheetData>
     <row r="1" s="1" customFormat="1" ht="13.5" spans="1:11">
       <c r="A1" s="3" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" ht="247" spans="1:7">
       <c r="A2" s="2" t="s">
-        <v>414</v>
+        <v>418</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>415</v>
+        <v>419</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>416</v>
+        <v>420</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>417</v>
+        <v>421</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>418</v>
+        <v>422</v>
       </c>
     </row>
     <row r="3" ht="260" spans="1:7">
       <c r="A3" s="2" t="s">
+        <v>423</v>
+      </c>
+      <c r="B3" s="4" t="s">
         <v>419</v>
       </c>
-      <c r="B3" s="4" t="s">
-        <v>415</v>
-      </c>
       <c r="C3" s="5" t="s">
-        <v>420</v>
+        <v>424</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>421</v>
+        <v>425</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>422</v>
-      </c>
-    </row>
-    <row r="4" ht="91" spans="1:7">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="4" ht="117" spans="1:7">
       <c r="A4" s="2" t="s">
-        <v>423</v>
+        <v>427</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>415</v>
+        <v>419</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>424</v>
+        <v>428</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>425</v>
+        <v>429</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>426</v>
-      </c>
-    </row>
-    <row r="5" ht="43.5" spans="1:2">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="5" ht="130" spans="1:7">
       <c r="A5" s="2" t="s">
-        <v>427</v>
+        <v>431</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>415</v>
-      </c>
-    </row>
-    <row r="6" ht="43.5" spans="1:2">
+        <v>419</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>432</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>166</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>433</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="6" ht="130" spans="1:7">
       <c r="A6" s="2" t="s">
-        <v>428</v>
+        <v>435</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>415</v>
-      </c>
-    </row>
-    <row r="7" ht="43.5" spans="1:2">
+        <v>419</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>436</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>166</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>437</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="7" ht="247" spans="1:7">
       <c r="A7" s="2" t="s">
-        <v>429</v>
+        <v>439</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>415</v>
-      </c>
-    </row>
-    <row r="8" ht="43.5" spans="1:2">
-      <c r="A8" s="2" t="s">
-        <v>430</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>415</v>
-      </c>
-    </row>
-    <row r="9" ht="43.5" spans="1:2">
-      <c r="A9" s="2" t="s">
-        <v>431</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>415</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1">
-      <c r="A10" s="2" t="s">
-        <v>432</v>
-      </c>
+        <v>419</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>440</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>166</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>441</v>
+      </c>
+      <c r="G7" s="7" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="8" spans="2:2">
+      <c r="B8" s="4"/>
+    </row>
+    <row r="9" spans="2:2">
+      <c r="B9" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>